<commit_message>
Exercise 2b - Parametrización
</commit_message>
<xml_diff>
--- a/DemoExerciseDay2/Default.xlsx
+++ b/DemoExerciseDay2/Default.xlsx
@@ -8,10 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="Action1" sheetId="2" r:id="rId2"/>
+    <sheet name="ExcerciseDay2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+  <si>
+    <t>p_Text</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -154,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -162,15 +170,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,16 +504,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.41796875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" s="4" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -490,12 +549,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>